<commit_message>
Updates documentation of gene panels. Relates to #595
</commit_message>
<xml_diff>
--- a/docs/static/scout-3-panel-file-example.xlsx
+++ b/docs/static/scout-3-panel-file-example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7600" yWindow="620" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -21,24 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>HGNC_symbol</t>
-  </si>
-  <si>
-    <t>HGNC_IDnumber</t>
-  </si>
-  <si>
-    <t>Disease_associated_transcript</t>
-  </si>
-  <si>
-    <t>Mosaicism</t>
-  </si>
-  <si>
-    <t>Reduced_penetrance</t>
-  </si>
-  <si>
-    <t>Genetic_disease_model</t>
-  </si>
-  <si>
     <t>ADK</t>
   </si>
   <si>
@@ -51,10 +33,28 @@
     <t>NM_006721.3,NM_001123</t>
   </si>
   <si>
-    <t>Database_entry_version</t>
-  </si>
-  <si>
     <t>10.5</t>
+  </si>
+  <si>
+    <t>hgnc_id</t>
+  </si>
+  <si>
+    <t>hgnc_symbol</t>
+  </si>
+  <si>
+    <t>disease_associated_transcripts</t>
+  </si>
+  <si>
+    <t>genetic_disease_models</t>
+  </si>
+  <si>
+    <t>mosaicism</t>
+  </si>
+  <si>
+    <t>reduced_penetrance</t>
+  </si>
+  <si>
+    <t>database_entry_version</t>
   </si>
 </sst>
 </file>
@@ -474,32 +474,32 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -507,19 +507,19 @@
         <v>257</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Document panel loading"
</commit_message>
<xml_diff>
--- a/docs/static/scout-3-panel-file-example.xlsx
+++ b/docs/static/scout-3-panel-file-example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7600" yWindow="620" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -21,6 +21,24 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
+    <t>HGNC_symbol</t>
+  </si>
+  <si>
+    <t>HGNC_IDnumber</t>
+  </si>
+  <si>
+    <t>Disease_associated_transcript</t>
+  </si>
+  <si>
+    <t>Mosaicism</t>
+  </si>
+  <si>
+    <t>Reduced_penetrance</t>
+  </si>
+  <si>
+    <t>Genetic_disease_model</t>
+  </si>
+  <si>
     <t>ADK</t>
   </si>
   <si>
@@ -33,28 +51,10 @@
     <t>NM_006721.3,NM_001123</t>
   </si>
   <si>
+    <t>Database_entry_version</t>
+  </si>
+  <si>
     <t>10.5</t>
-  </si>
-  <si>
-    <t>hgnc_id</t>
-  </si>
-  <si>
-    <t>hgnc_symbol</t>
-  </si>
-  <si>
-    <t>disease_associated_transcripts</t>
-  </si>
-  <si>
-    <t>genetic_disease_models</t>
-  </si>
-  <si>
-    <t>mosaicism</t>
-  </si>
-  <si>
-    <t>reduced_penetrance</t>
-  </si>
-  <si>
-    <t>database_entry_version</t>
   </si>
 </sst>
 </file>
@@ -474,32 +474,32 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -507,19 +507,19 @@
         <v>257</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates documentation on gene panels
</commit_message>
<xml_diff>
--- a/docs/static/scout-3-panel-file-example.xlsx
+++ b/docs/static/scout-3-panel-file-example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="7600" yWindow="620" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -21,24 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>HGNC_symbol</t>
-  </si>
-  <si>
-    <t>HGNC_IDnumber</t>
-  </si>
-  <si>
-    <t>Disease_associated_transcript</t>
-  </si>
-  <si>
-    <t>Mosaicism</t>
-  </si>
-  <si>
-    <t>Reduced_penetrance</t>
-  </si>
-  <si>
-    <t>Genetic_disease_model</t>
-  </si>
-  <si>
     <t>ADK</t>
   </si>
   <si>
@@ -51,10 +33,28 @@
     <t>NM_006721.3,NM_001123</t>
   </si>
   <si>
-    <t>Database_entry_version</t>
-  </si>
-  <si>
     <t>10.5</t>
+  </si>
+  <si>
+    <t>hgnc_id</t>
+  </si>
+  <si>
+    <t>hgnc_symbol</t>
+  </si>
+  <si>
+    <t>disease_associated_transcripts</t>
+  </si>
+  <si>
+    <t>genetic_disease_models</t>
+  </si>
+  <si>
+    <t>mosaicism</t>
+  </si>
+  <si>
+    <t>reduced_penetrance</t>
+  </si>
+  <si>
+    <t>database_entry_version</t>
   </si>
 </sst>
 </file>
@@ -474,32 +474,32 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -507,19 +507,19 @@
         <v>257</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>